<commit_message>
More category work, including Platforms conversion task
</commit_message>
<xml_diff>
--- a/category_renaming.xlsx
+++ b/category_renaming.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9900" yWindow="300" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="600" yWindow="900" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="114">
   <si>
     <t>and iPad Pro</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Tabletop</t>
   </si>
   <si>
-    <t>macOS</t>
-  </si>
-  <si>
     <t>Windows</t>
   </si>
   <si>
@@ -201,9 +198,6 @@
     <t>biodiversity</t>
   </si>
   <si>
-    <t>cell biology</t>
-  </si>
-  <si>
     <t>cells</t>
   </si>
   <si>
@@ -252,9 +246,6 @@
     <t>high school</t>
   </si>
   <si>
-    <t>?????</t>
-  </si>
-  <si>
     <t>history</t>
   </si>
   <si>
@@ -270,9 +261,6 @@
     <t>middle school</t>
   </si>
   <si>
-    <t>??????</t>
-  </si>
-  <si>
     <t>molecular science</t>
   </si>
   <si>
@@ -330,9 +318,6 @@
     <t>middle school, high school</t>
   </si>
   <si>
-    <t>elementary, school, middle school, high school, college</t>
-  </si>
-  <si>
     <t>DEVELOPER TYPES</t>
   </si>
   <si>
@@ -373,6 +358,9 @@
   </si>
   <si>
     <t>??</t>
+  </si>
+  <si>
+    <t>elementary school, middle school, high school, college</t>
   </si>
 </sst>
 </file>
@@ -429,8 +417,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -443,13 +439,21 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -781,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -793,7 +797,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -897,7 +901,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -905,7 +909,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -913,7 +917,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -934,489 +938,477 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C33" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" t="s">
-        <v>76</v>
-      </c>
-      <c r="C45" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" t="s">
-        <v>82</v>
-      </c>
-      <c r="C50" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C54" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C56" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B60" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B61" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B62" t="s">
         <v>98</v>
-      </c>
-      <c r="B62" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B63" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B64" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B65" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B66" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B67" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B68" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B69" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B70" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B73" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B74" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B75" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C75" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B76" t="s">
         <v>108</v>
-      </c>
-      <c r="B76" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B77" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B78" t="s">
+        <v>109</v>
+      </c>
+      <c r="C78" t="s">
         <v>110</v>
-      </c>
-      <c r="B78" t="s">
-        <v>114</v>
-      </c>
-      <c r="C78" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B79" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C79" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B80" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>